<commit_message>
Adds BOM, changes Pick and Place, and fixes component footprints
</commit_message>
<xml_diff>
--- a/Buck_Converter/Pick Place for Buck_PCB.xlsx
+++ b/Buck_Converter/Pick Place for Buck_PCB.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\Waterloop\electrical-BMS\Buck_Converter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067EF5A0-349C-4EF5-BC74-86B1E90D0383}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{716B3A16-BF67-4EA3-9EAF-E95EAFFF09A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Pick Place for Buck_PCB" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t>Designator</t>
   </si>
@@ -34,7 +34,79 @@
     <t>Rotation</t>
   </si>
   <si>
+    <t>C1</t>
+  </si>
+  <si>
     <t>TopLayer</t>
+  </si>
+  <si>
+    <t>1210_-_Capacitor</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>0805_-_Capacitor</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>OCVZ0606_-_CAPACITOR</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>SMA_-_DIODE</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>MSS1210_-_INDUCTOR</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>HDR1X2</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>0603_-_Resistor</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>0805_-_Resistor</t>
+  </si>
+  <si>
+    <t>R4</t>
   </si>
   <si>
     <t>U1</t>
@@ -52,7 +124,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -886,20 +958,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -907,39 +978,359 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="D2">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="E2">
+        <v>22.225000000000001</v>
+      </c>
+      <c r="F2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>26.161999999999999</v>
+      </c>
+      <c r="E3">
+        <v>12.664</v>
+      </c>
+      <c r="F3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>19.05</v>
+      </c>
+      <c r="E4">
+        <v>22.986999999999998</v>
+      </c>
+      <c r="F4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>16.763999999999999</v>
+      </c>
+      <c r="E5">
+        <v>12.954000000000001</v>
+      </c>
+      <c r="F5">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>15.875</v>
+      </c>
+      <c r="E6">
+        <v>17.399000000000001</v>
+      </c>
+      <c r="F6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>10.2498</v>
+      </c>
+      <c r="E7">
+        <v>16.890999999999998</v>
+      </c>
+      <c r="F7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>24.638000000000002</v>
+      </c>
+      <c r="E8">
+        <v>22.986999999999998</v>
+      </c>
+      <c r="F8">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>32.003999999999998</v>
+      </c>
+      <c r="E9">
+        <v>9.7789999999999999</v>
+      </c>
+      <c r="F9">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>28.342300000000002</v>
+      </c>
+      <c r="E10">
+        <v>19.812000000000001</v>
+      </c>
+      <c r="F10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>38.734999999999999</v>
+      </c>
+      <c r="E11">
+        <v>21.971</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12">
+        <v>12.192</v>
+      </c>
+      <c r="E12">
+        <v>23.114000000000001</v>
+      </c>
+      <c r="F12">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13">
+        <v>38.353999999999999</v>
+      </c>
+      <c r="E13">
+        <v>11.048999999999999</v>
+      </c>
+      <c r="F13">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14">
+        <v>13.9208</v>
+      </c>
+      <c r="E14">
+        <v>14.478</v>
+      </c>
+      <c r="F14">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>12.954000000000001</v>
+      </c>
+      <c r="E15">
+        <v>18.161000000000001</v>
+      </c>
+      <c r="F15">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16">
+        <v>20.574000000000002</v>
+      </c>
+      <c r="E16">
+        <v>10.541</v>
+      </c>
+      <c r="F16">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17">
+        <v>12.2165</v>
+      </c>
+      <c r="E17">
+        <v>14.478</v>
+      </c>
+      <c r="F17">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18">
         <v>21.032800000000002</v>
       </c>
-      <c r="D2">
+      <c r="E18">
         <v>17.78</v>
       </c>
-      <c r="E2">
+      <c r="F18">
         <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes Outjob for JLCPCB
</commit_message>
<xml_diff>
--- a/Buck_Converter/Pick Place for Buck_PCB.xlsx
+++ b/Buck_Converter/Pick Place for Buck_PCB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\Waterloop\electrical-BMS\Buck_Converter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{716B3A16-BF67-4EA3-9EAF-E95EAFFF09A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E9DD69EB-19A1-47DF-A209-34426CDDA763}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="4752" yWindow="4020" windowWidth="13920" windowHeight="7572"/>
   </bookViews>
   <sheets>
     <sheet name="Pick Place for Buck_PCB" sheetId="1" r:id="rId1"/>
@@ -20,27 +20,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
   <si>
     <t>Designator</t>
   </si>
   <si>
+    <t>Footprint</t>
+  </si>
+  <si>
     <t>Layer</t>
   </si>
   <si>
-    <t>Footprint</t>
-  </si>
-  <si>
     <t>Rotation</t>
   </si>
   <si>
+    <t>Comment</t>
+  </si>
+  <si>
     <t>C1</t>
   </si>
   <si>
+    <t>1210_-_Capacitor</t>
+  </si>
+  <si>
     <t>TopLayer</t>
   </si>
   <si>
-    <t>1210_-_Capacitor</t>
+    <t>Cin</t>
   </si>
   <si>
     <t>C2</t>
@@ -49,45 +55,75 @@
     <t>0805_-_Capacitor</t>
   </si>
   <si>
+    <t>Css</t>
+  </si>
+  <si>
     <t>C3</t>
   </si>
   <si>
+    <t>Cbyp</t>
+  </si>
+  <si>
     <t>C4</t>
   </si>
   <si>
+    <t>Cramp</t>
+  </si>
+  <si>
     <t>C5</t>
   </si>
   <si>
+    <t>Ccomp2</t>
+  </si>
+  <si>
     <t>C6</t>
   </si>
   <si>
+    <t>Ccomp1</t>
+  </si>
+  <si>
     <t>C7</t>
   </si>
   <si>
+    <t>Cboot</t>
+  </si>
+  <si>
     <t>C8</t>
   </si>
   <si>
     <t>OCVZ0606_-_CAPACITOR</t>
   </si>
   <si>
+    <t>Cout</t>
+  </si>
+  <si>
     <t>D1</t>
   </si>
   <si>
     <t>SMA_-_DIODE</t>
   </si>
   <si>
+    <t>Diode - Schottky</t>
+  </si>
+  <si>
     <t>L1</t>
   </si>
   <si>
     <t>MSS1210_-_INDUCTOR</t>
   </si>
   <si>
+    <t>Inductor</t>
+  </si>
+  <si>
     <t>P1</t>
   </si>
   <si>
     <t>HDR1X2</t>
   </si>
   <si>
+    <t>1x2 Header</t>
+  </si>
+  <si>
     <t>P2</t>
   </si>
   <si>
@@ -97,28 +133,52 @@
     <t>0603_-_Resistor</t>
   </si>
   <si>
+    <t>Rt</t>
+  </si>
+  <si>
     <t>R2</t>
   </si>
   <si>
+    <t>Rcomp</t>
+  </si>
+  <si>
     <t>R3</t>
   </si>
   <si>
     <t>0805_-_Resistor</t>
   </si>
   <si>
+    <t>Rfb2</t>
+  </si>
+  <si>
     <t>R4</t>
   </si>
   <si>
+    <t>Rfb1</t>
+  </si>
+  <si>
     <t>U1</t>
   </si>
   <si>
     <t>LM5005</t>
   </si>
   <si>
-    <t>Center X</t>
-  </si>
-  <si>
-    <t>Center Y</t>
+    <t>Mid X</t>
+  </si>
+  <si>
+    <t>Mid Y</t>
+  </si>
+  <si>
+    <t>Ref X</t>
+  </si>
+  <si>
+    <t>Ref Y</t>
+  </si>
+  <si>
+    <t>Pad X</t>
+  </si>
+  <si>
+    <t>Pad Y</t>
   </si>
 </sst>
 </file>
@@ -959,21 +1019,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -981,356 +1040,626 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>15.113</v>
+      </c>
+      <c r="D2">
+        <v>21.844000000000001</v>
+      </c>
+      <c r="E2">
+        <v>15.113</v>
+      </c>
+      <c r="F2">
+        <v>21.844000000000001</v>
+      </c>
+      <c r="G2">
+        <v>15.113</v>
+      </c>
+      <c r="H2">
+        <v>23.369</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2">
+        <v>270</v>
+      </c>
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>26.161999999999999</v>
+      </c>
+      <c r="D3">
+        <v>12.664</v>
+      </c>
+      <c r="E3">
+        <v>26.161999999999999</v>
+      </c>
+      <c r="F3">
+        <v>12.664</v>
+      </c>
+      <c r="G3">
+        <v>26.161999999999999</v>
+      </c>
+      <c r="H3">
+        <v>11.739000000000001</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3">
+        <v>90</v>
+      </c>
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>19.05</v>
+      </c>
+      <c r="D4">
+        <v>22.986999999999998</v>
+      </c>
+      <c r="E4">
+        <v>19.05</v>
+      </c>
+      <c r="F4">
+        <v>22.986999999999998</v>
+      </c>
+      <c r="G4">
+        <v>19.975000000000001</v>
+      </c>
+      <c r="H4">
+        <v>22.986999999999998</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4">
+        <v>180</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>16.763999999999999</v>
+      </c>
+      <c r="D5">
+        <v>12.954000000000001</v>
+      </c>
+      <c r="E5">
+        <v>16.763999999999999</v>
+      </c>
+      <c r="F5">
+        <v>12.954000000000001</v>
+      </c>
+      <c r="G5">
+        <v>17.689</v>
+      </c>
+      <c r="H5">
+        <v>12.954000000000001</v>
+      </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5">
+        <v>180</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>15.875</v>
+      </c>
+      <c r="D6">
+        <v>17.399000000000001</v>
+      </c>
+      <c r="E6">
+        <v>15.875</v>
+      </c>
+      <c r="F6">
+        <v>17.399000000000001</v>
+      </c>
+      <c r="G6">
+        <v>15.875</v>
+      </c>
+      <c r="H6">
+        <v>16.474</v>
+      </c>
+      <c r="I6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <v>90</v>
+      </c>
+      <c r="K6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>10.2498</v>
+      </c>
+      <c r="D7">
+        <v>16.890999999999998</v>
+      </c>
+      <c r="E7">
+        <v>10.2498</v>
+      </c>
+      <c r="F7">
+        <v>16.890999999999998</v>
+      </c>
+      <c r="G7">
+        <v>10.2498</v>
+      </c>
+      <c r="H7">
+        <v>15.965999999999999</v>
+      </c>
+      <c r="I7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>90</v>
+      </c>
+      <c r="K7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>24.638000000000002</v>
+      </c>
+      <c r="D8">
+        <v>22.986999999999998</v>
+      </c>
+      <c r="E8">
+        <v>24.638000000000002</v>
+      </c>
+      <c r="F8">
+        <v>22.986999999999998</v>
+      </c>
+      <c r="G8">
+        <v>25.562999999999999</v>
+      </c>
+      <c r="H8">
+        <v>22.986999999999998</v>
+      </c>
+      <c r="I8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <v>180</v>
+      </c>
+      <c r="K8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>32.003999999999998</v>
+      </c>
+      <c r="D9">
+        <v>9.7789999999999999</v>
+      </c>
+      <c r="E9">
+        <v>32.003999999999998</v>
+      </c>
+      <c r="F9">
+        <v>9.7789999999999999</v>
+      </c>
+      <c r="G9">
+        <v>32.003999999999998</v>
+      </c>
+      <c r="H9">
+        <v>12.404</v>
+      </c>
+      <c r="I9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9">
+        <v>270</v>
+      </c>
+      <c r="K9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10">
+        <v>28.342300000000002</v>
+      </c>
+      <c r="D10">
+        <v>19.812000000000001</v>
+      </c>
+      <c r="E10">
+        <v>28.342300000000002</v>
+      </c>
+      <c r="F10">
+        <v>19.812000000000001</v>
+      </c>
+      <c r="G10">
+        <v>28.342300000000002</v>
+      </c>
+      <c r="H10">
+        <v>18.212</v>
+      </c>
+      <c r="I10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10">
+        <v>90</v>
+      </c>
+      <c r="K10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11">
+        <v>38.734999999999999</v>
+      </c>
+      <c r="D11">
+        <v>21.971</v>
+      </c>
+      <c r="E11">
+        <v>38.734999999999999</v>
+      </c>
+      <c r="F11">
+        <v>21.971</v>
+      </c>
+      <c r="G11">
+        <v>33.984999999999999</v>
+      </c>
+      <c r="H11">
+        <v>21.971</v>
+      </c>
+      <c r="I11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>31</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>15.747999999999999</v>
-      </c>
-      <c r="E2">
-        <v>22.225000000000001</v>
-      </c>
-      <c r="F2">
+      <c r="C12">
+        <v>11.4328</v>
+      </c>
+      <c r="D12">
+        <v>23.114000000000001</v>
+      </c>
+      <c r="E12">
+        <v>11.4328</v>
+      </c>
+      <c r="F12">
+        <v>24.384</v>
+      </c>
+      <c r="G12">
+        <v>11.4328</v>
+      </c>
+      <c r="H12">
+        <v>24.384</v>
+      </c>
+      <c r="I12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12">
         <v>270</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="K12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <v>38.353999999999999</v>
+      </c>
+      <c r="D13">
+        <v>11.048999999999999</v>
+      </c>
+      <c r="E13">
+        <v>38.353999999999999</v>
+      </c>
+      <c r="F13">
+        <v>12.319000000000001</v>
+      </c>
+      <c r="G13">
+        <v>38.353999999999999</v>
+      </c>
+      <c r="H13">
+        <v>12.319000000000001</v>
+      </c>
+      <c r="I13" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>26.161999999999999</v>
-      </c>
-      <c r="E3">
-        <v>12.664</v>
-      </c>
-      <c r="F3">
+      <c r="J13">
+        <v>270</v>
+      </c>
+      <c r="K13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14">
+        <v>13.9208</v>
+      </c>
+      <c r="D14">
+        <v>14.478</v>
+      </c>
+      <c r="E14">
+        <v>13.9208</v>
+      </c>
+      <c r="F14">
+        <v>14.478</v>
+      </c>
+      <c r="G14">
+        <v>13.9208</v>
+      </c>
+      <c r="H14">
+        <v>13.653</v>
+      </c>
+      <c r="I14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14">
         <v>90</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>19.05</v>
-      </c>
-      <c r="E4">
-        <v>22.986999999999998</v>
-      </c>
-      <c r="F4">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>16.763999999999999</v>
-      </c>
-      <c r="E5">
+      <c r="K14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15">
         <v>12.954000000000001</v>
       </c>
-      <c r="F5">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>15.875</v>
-      </c>
-      <c r="E6">
-        <v>17.399000000000001</v>
-      </c>
-      <c r="F6">
+      <c r="D15">
+        <v>18.161000000000001</v>
+      </c>
+      <c r="E15">
+        <v>12.954000000000001</v>
+      </c>
+      <c r="F15">
+        <v>18.161000000000001</v>
+      </c>
+      <c r="G15">
+        <v>12.129</v>
+      </c>
+      <c r="H15">
+        <v>18.161000000000001</v>
+      </c>
+      <c r="I15" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15">
+        <v>360</v>
+      </c>
+      <c r="K15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16">
+        <v>20.574000000000002</v>
+      </c>
+      <c r="D16">
+        <v>10.032999999999999</v>
+      </c>
+      <c r="E16">
+        <v>20.574000000000002</v>
+      </c>
+      <c r="F16">
+        <v>10.032999999999999</v>
+      </c>
+      <c r="G16">
+        <v>19.574000000000002</v>
+      </c>
+      <c r="H16">
+        <v>10.032999999999999</v>
+      </c>
+      <c r="I16" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16">
+        <v>360</v>
+      </c>
+      <c r="K16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17">
+        <v>12.2165</v>
+      </c>
+      <c r="D17">
+        <v>14.478</v>
+      </c>
+      <c r="E17">
+        <v>12.2165</v>
+      </c>
+      <c r="F17">
+        <v>14.478</v>
+      </c>
+      <c r="G17">
+        <v>12.2165</v>
+      </c>
+      <c r="H17">
+        <v>13.478</v>
+      </c>
+      <c r="I17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>10.2498</v>
-      </c>
-      <c r="E7">
-        <v>16.890999999999998</v>
-      </c>
-      <c r="F7">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>24.638000000000002</v>
-      </c>
-      <c r="E8">
-        <v>22.986999999999998</v>
-      </c>
-      <c r="F8">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9">
-        <v>32.003999999999998</v>
-      </c>
-      <c r="E9">
-        <v>9.7789999999999999</v>
-      </c>
-      <c r="F9">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10">
-        <v>28.342300000000002</v>
-      </c>
-      <c r="E10">
-        <v>19.812000000000001</v>
-      </c>
-      <c r="F10">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11">
-        <v>38.734999999999999</v>
-      </c>
-      <c r="E11">
-        <v>21.971</v>
-      </c>
-      <c r="F11">
+      <c r="K17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18">
+        <v>21.032800000000002</v>
+      </c>
+      <c r="D18">
+        <v>17.78</v>
+      </c>
+      <c r="E18">
+        <v>21.032800000000002</v>
+      </c>
+      <c r="F18">
+        <v>17.78</v>
+      </c>
+      <c r="G18">
+        <v>18.082799999999999</v>
+      </c>
+      <c r="H18">
+        <v>20.704999999999998</v>
+      </c>
+      <c r="I18" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12">
-        <v>12.192</v>
-      </c>
-      <c r="E12">
-        <v>23.114000000000001</v>
-      </c>
-      <c r="F12">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13">
-        <v>38.353999999999999</v>
-      </c>
-      <c r="E13">
-        <v>11.048999999999999</v>
-      </c>
-      <c r="F13">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14">
-        <v>13.9208</v>
-      </c>
-      <c r="E14">
-        <v>14.478</v>
-      </c>
-      <c r="F14">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15">
-        <v>12.954000000000001</v>
-      </c>
-      <c r="E15">
-        <v>18.161000000000001</v>
-      </c>
-      <c r="F15">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16">
-        <v>20.574000000000002</v>
-      </c>
-      <c r="E16">
-        <v>10.541</v>
-      </c>
-      <c r="F16">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17">
-        <v>12.2165</v>
-      </c>
-      <c r="E17">
-        <v>14.478</v>
-      </c>
-      <c r="F17">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18">
-        <v>21.032800000000002</v>
-      </c>
-      <c r="E18">
-        <v>17.78</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
+      <c r="K18" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>